<commit_message>
q 1-6 added bar chart
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgood\Documents\nss_data_analytics\projects\lookups-budget-marthahunter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD85446-8EBE-46B8-AE8A-BCDAFCE2B102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344E55A7-D4A9-49E8-BFB8-44DA78B32509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,7 +315,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,8 +462,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +657,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -813,7 +827,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +850,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1"/>
+    <xf numFmtId="43" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,6 +921,1103 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Projected vs. Actual Budget</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Budget</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:shade val="76000"/>
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5847800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6223700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6207300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0ABC-4C95-9D00-A939F11F3DD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:tint val="77000"/>
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5772288.3300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5909077.9399999902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6056976.6699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0ABC-4C95-9D00-A939F11F3DD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="2113971423"/>
+        <c:axId val="2114778655"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2113971423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2114778655"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2114778655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2113971423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent6">
+        <a:lumMod val="40000"/>
+        <a:lumOff val="60000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A1F8BB1-3473-FF49-7770-9ACD89EE5E2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1197,7 +2320,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4337,6 +5460,13 @@
         <f t="shared" ref="D57:D61" si="11">VLOOKUP($A57,$A$1:$P$52, 14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="18"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
@@ -4354,6 +5484,13 @@
         <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="18"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
@@ -4371,8 +5508,18 @@
         <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="E59" s="18"/>
+      <c r="F59" s="16" t="str">
+        <f>B82</f>
+        <v>Criminal Court Clerk</v>
+      </c>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="18"/>
+    </row>
+    <row r="60" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -4388,8 +5535,15 @@
         <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="E60" s="18"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="18"/>
+    </row>
+    <row r="61" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -4405,11 +5559,25 @@
         <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
+      <c r="E61" s="18"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="18"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="18"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A63" s="6" t="s">
@@ -4418,6 +5586,13 @@
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="18"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
@@ -4432,8 +5607,15 @@
       <c r="D64" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="18"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -4449,8 +5631,15 @@
         <f>_xlfn.XLOOKUP($A65,$A$2:$A$52, N$2:N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="18"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -4466,8 +5655,15 @@
         <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP($A66,$A$2:$A$52, N$2:N$52)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="18"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -4483,8 +5679,15 @@
         <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="18"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -4500,8 +5703,15 @@
         <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="18"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -4517,8 +5727,15 @@
         <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="18"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4534,21 +5751,42 @@
         <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="18"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="18"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="18"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4561,8 +5799,15 @@
       <c r="D73" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="18"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -4578,8 +5823,15 @@
         <f>INDEX(N$2:N$52,MATCH($A74, $A$2:$A$52, 0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="18"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -4595,8 +5847,15 @@
         <f t="shared" ref="D75:D79" si="17">INDEX(N$2:N$52,MATCH($A75, $A$2:$A$52, 0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="18"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -4612,8 +5871,15 @@
         <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="18"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -4629,8 +5895,15 @@
         <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="20"/>
+      <c r="K77" s="18"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -4646,8 +5919,15 @@
         <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="18"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4663,73 +5943,147 @@
         <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="20"/>
+      <c r="K79" s="18"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="18"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="18"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>0</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
+      <c r="J82" s="20"/>
+      <c r="K82" s="18"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B83" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="20"/>
+      <c r="K83" s="18"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>73</v>
       </c>
       <c r="B84" s="8">
         <f>INDEX($B$2:$B$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>356640100</v>
+        <v>5847800</v>
       </c>
       <c r="C84" s="8">
         <f>INDEX($C$2:$C$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>341243679.13</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5772288.3300000001</v>
+      </c>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="19"/>
+      <c r="I84" s="19"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="18"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>74</v>
       </c>
       <c r="B85" s="8">
         <f>INDEX($G$2:$G$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>382685200</v>
+        <v>6223700</v>
       </c>
       <c r="C85" s="8">
         <f>INDEX($H$2:H$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>346340810.81999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5909077.9399999902</v>
+      </c>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+      <c r="I85" s="19"/>
+      <c r="J85" s="20"/>
+      <c r="K85" s="18"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>75</v>
       </c>
       <c r="B86" s="8">
         <f>INDEX($L$2:$L$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>376548600</v>
+        <v>6207300</v>
       </c>
       <c r="C86" s="8">
         <f>INDEX($M$2:$M$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>355279492.22999901</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6056976.6699999999</v>
+      </c>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="18"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="20"/>
+      <c r="K87" s="18"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="18"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -4745,7 +6099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B90" s="11" t="s">
         <v>0</v>
       </c>
@@ -4765,30 +6119,30 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>73</v>
       </c>
       <c r="E91" s="5"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>74</v>
       </c>
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>75</v>
       </c>
       <c r="E93" s="5"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -4843,6 +6197,9 @@
       <c r="E100" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F59:J60"/>
+  </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
@@ -4853,6 +6210,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
q 1-6 complete, fixed table formatting
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgood\Documents\nss_data_analytics\projects\lookups-budget-marthahunter\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344E55A7-D4A9-49E8-BFB8-44DA78B32509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B5BFF-077F-442E-BA69-E0E8A016198F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,7 +664,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -779,6 +779,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -827,7 +922,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -850,18 +945,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1"/>
-    <xf numFmtId="43" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="34" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="34" borderId="0" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="14" xfId="44" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="34" borderId="18" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="16" fillId="34" borderId="18" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,13 +1231,13 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5847800</c:v>
+                  <c:v>1552100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6223700</c:v>
+                  <c:v>1590700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6207300</c:v>
+                  <c:v>1579300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,13 +1362,13 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5772288.3300000001</c:v>
+                  <c:v>1315623.30999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5909077.9399999902</c:v>
+                  <c:v>1383905.98999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6056976.6699999999</c:v>
+                  <c:v>1337735.3199999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,15 +2102,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:colOff>1114426</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2319,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5460,15 +5578,12 @@
         <f t="shared" ref="D57:D61" si="11">VLOOKUP($A57,$A$1:$P$52, 14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="18"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -5484,13 +5599,10 @@
         <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="18"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="17"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
@@ -5508,16 +5620,14 @@
         <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="16" t="str">
+      <c r="F59" s="18" t="str">
         <f>B82</f>
-        <v>Criminal Court Clerk</v>
-      </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="18"/>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="20"/>
     </row>
     <row r="60" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
@@ -5535,13 +5645,11 @@
         <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-      <c r="K60" s="18"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="23"/>
     </row>
     <row r="61" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
@@ -5559,25 +5667,21 @@
         <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="E61" s="18"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="20"/>
-      <c r="K61" s="18"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="30"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="18"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="30"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A63" s="6" t="s">
@@ -5586,13 +5690,11 @@
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="18"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="30"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
@@ -5607,15 +5709,13 @@
       <c r="D64" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="18"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F64" s="31"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="30"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5631,15 +5731,13 @@
         <f>_xlfn.XLOOKUP($A65,$A$2:$A$52, N$2:N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="20"/>
-      <c r="K65" s="18"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F65" s="31"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="30"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -5655,15 +5753,13 @@
         <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP($A66,$A$2:$A$52, N$2:N$52)</f>
         <v>-311228.08999999997</v>
       </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="20"/>
-      <c r="K66" s="18"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F66" s="31"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="30"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -5679,15 +5775,13 @@
         <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="20"/>
-      <c r="K67" s="18"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F67" s="31"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="30"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -5703,15 +5797,13 @@
         <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="20"/>
-      <c r="K68" s="18"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F68" s="31"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="30"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -5727,15 +5819,13 @@
         <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="20"/>
-      <c r="K69" s="18"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F69" s="31"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="30"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -5751,42 +5841,36 @@
         <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="19"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="18"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F70" s="31"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="30"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
-      <c r="J71" s="20"/>
-      <c r="K71" s="18"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F71" s="31"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="30"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
-      <c r="J72" s="20"/>
-      <c r="K72" s="18"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F72" s="31"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="30"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5799,15 +5883,13 @@
       <c r="D73" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="20"/>
-      <c r="K73" s="18"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F73" s="31"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="30"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5823,15 +5905,13 @@
         <f>INDEX(N$2:N$52,MATCH($A74, $A$2:$A$52, 0))</f>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
-      <c r="J74" s="20"/>
-      <c r="K74" s="18"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F74" s="31"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="30"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -5847,15 +5927,13 @@
         <f t="shared" ref="D75:D79" si="17">INDEX(N$2:N$52,MATCH($A75, $A$2:$A$52, 0))</f>
         <v>-311228.08999999997</v>
       </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
-      <c r="J75" s="20"/>
-      <c r="K75" s="18"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F75" s="31"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="30"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -5871,15 +5949,13 @@
         <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="20"/>
-      <c r="K76" s="18"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F76" s="31"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="30"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -5895,15 +5971,13 @@
         <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="20"/>
-      <c r="K77" s="18"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F77" s="31"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="30"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -5919,15 +5993,13 @@
         <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="20"/>
-      <c r="K78" s="18"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F78" s="31"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="30"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -5943,147 +6015,128 @@
         <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="20"/>
-      <c r="K79" s="18"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="20"/>
-      <c r="K80" s="18"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F79" s="31"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="30"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F80" s="31"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="30"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
-      <c r="J81" s="20"/>
-      <c r="K81" s="18"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F81" s="31"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="30"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-      <c r="J82" s="20"/>
-      <c r="K82" s="18"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B83" s="9" t="s">
+      <c r="B82" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="34"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
+      <c r="J82" s="30"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B83" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
-      <c r="J83" s="20"/>
-      <c r="K83" s="18"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F83" s="31"/>
+      <c r="G83" s="29"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="30"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B84" s="32">
         <f>INDEX($B$2:$B$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>5847800</v>
-      </c>
-      <c r="C84" s="8">
+        <v>1552100</v>
+      </c>
+      <c r="C84" s="32">
         <f>INDEX($C$2:$C$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>5772288.3300000001</v>
-      </c>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="19"/>
-      <c r="H84" s="19"/>
-      <c r="I84" s="19"/>
-      <c r="J84" s="20"/>
-      <c r="K84" s="18"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1315623.30999999</v>
+      </c>
+      <c r="F84" s="31"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="30"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="32">
         <f>INDEX($G$2:$G$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>6223700</v>
-      </c>
-      <c r="C85" s="8">
+        <v>1590700</v>
+      </c>
+      <c r="C85" s="32">
         <f>INDEX($H$2:H$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>5909077.9399999902</v>
-      </c>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="19"/>
-      <c r="H85" s="19"/>
-      <c r="I85" s="19"/>
-      <c r="J85" s="20"/>
-      <c r="K85" s="18"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1383905.98999999</v>
+      </c>
+      <c r="F85" s="31"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="30"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="32">
         <f>INDEX($L$2:$L$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>6207300</v>
-      </c>
-      <c r="C86" s="8">
+        <v>1579300</v>
+      </c>
+      <c r="C86" s="32">
         <f>INDEX($M$2:$M$52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>6056976.6699999999</v>
-      </c>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="19"/>
-      <c r="H86" s="19"/>
-      <c r="I86" s="19"/>
-      <c r="J86" s="20"/>
-      <c r="K86" s="18"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="19"/>
-      <c r="H87" s="19"/>
-      <c r="I87" s="19"/>
-      <c r="J87" s="20"/>
-      <c r="K87" s="18"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1337735.3199999901</v>
+      </c>
+      <c r="F86" s="31"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="30"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F87" s="31"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="30"/>
+    </row>
+    <row r="88" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="20"/>
-      <c r="K88" s="18"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F88" s="24"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="26"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -6099,7 +6152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B90" s="11" t="s">
         <v>0</v>
       </c>
@@ -6119,30 +6172,30 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>73</v>
       </c>
       <c r="E91" s="5"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>74</v>
       </c>
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>75</v>
       </c>
       <c r="E93" s="5"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>77</v>
       </c>

</xml_diff>